<commit_message>
Cleaned up pytests - test_dialogs showing entries.
</commit_message>
<xml_diff>
--- a/tests/db/Case_Data.xlsx
+++ b/tests/db/Case_Data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:K501"/>
+  <dimension ref="A2:K525"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -23336,6 +23336,1094 @@
       <c r="I501" t="inlineStr">
         <is>
           <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F502" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G502" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H502" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I502" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E503" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F503" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G503" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H503" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I503" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E504" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F504" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G504" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H504" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I504" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F505" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G505" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H505" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I505" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F506" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G506" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H506" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I506" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J506" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K506" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H507" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I507" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J507" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K507" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F508" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G508" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H508" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I508" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J508" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K508" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F509" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G509" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H509" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I509" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J509" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K509" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F510" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F513" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F517" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I518" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H519" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I519" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H520" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H521" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F522" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H522" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J522" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K522" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I523" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J523" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K523" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H524" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I524" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J524" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K524" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H525" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I525" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J525" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K525" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed test_no_jail and moved nonrefactored to subfolder
</commit_message>
<xml_diff>
--- a/tests/db/Case_Data.xlsx
+++ b/tests/db/Case_Data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:K525"/>
+  <dimension ref="A2:K535"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -24424,6 +24424,476 @@
       <c r="K525" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H526" t="inlineStr">
+        <is>
+          <t>$ 50</t>
+        </is>
+      </c>
+      <c r="I526" t="inlineStr">
+        <is>
+          <t>$ 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H527" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I527" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F528" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H528" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I528" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F529" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G529" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H529" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I529" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>Speeding &gt; 25 mph</t>
+        </is>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>4511.21(B)(2)</t>
+        </is>
+      </c>
+      <c r="E530" t="inlineStr">
+        <is>
+          <t>Minor Misdemeanor</t>
+        </is>
+      </c>
+      <c r="F530" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G530" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H530" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I530" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>DUS UCM</t>
+        </is>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E531" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F531" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G531" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H531" t="inlineStr">
+        <is>
+          <t>$ 50</t>
+        </is>
+      </c>
+      <c r="I531" t="inlineStr">
+        <is>
+          <t>$ 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>OPERATING W/O A VALID OL - UCM</t>
+        </is>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F532" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G532" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H532" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I532" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>FAILURE TO REINSTATE LICENSE UCM 1-2/3YRS</t>
+        </is>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F533" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G533" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H533" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I533" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>FAILURE TO FILE REGISTRATION</t>
+        </is>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F534" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G534" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H534" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I534" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>Speeding &gt; 25 mph</t>
+        </is>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>4511.21(B)(2)</t>
+        </is>
+      </c>
+      <c r="E535" t="inlineStr">
+        <is>
+          <t>Minor Misdemeanor</t>
+        </is>
+      </c>
+      <c r="F535" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G535" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H535" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I535" t="inlineStr">
+        <is>
+          <t>$ 0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated tests for fine only.
</commit_message>
<xml_diff>
--- a/tests/db/Case_Data.xlsx
+++ b/tests/db/Case_Data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:K1394"/>
+  <dimension ref="A2:K1410"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -67952,6 +67952,838 @@
         </is>
       </c>
       <c r="K1394" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>DUS Ucm</t>
+        </is>
+      </c>
+      <c r="D1395" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E1395" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1395" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1395" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1395" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1395" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>Operating W/o A Valid Ol - Ucm</t>
+        </is>
+      </c>
+      <c r="D1396" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E1396" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1396" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1396" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1396" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1396" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>Failure To Reinstate License Ucm 1-2/3yrs</t>
+        </is>
+      </c>
+      <c r="D1397" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E1397" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1397" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1397" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1397" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1397" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>Failure To File Registration</t>
+        </is>
+      </c>
+      <c r="D1398" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E1398" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F1398" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1398" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1398" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1398" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>DUS Ucm</t>
+        </is>
+      </c>
+      <c r="D1399" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E1399" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1399" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1399" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1399" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1399" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1399" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1399" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>Operating W/o A Valid Ol - Ucm</t>
+        </is>
+      </c>
+      <c r="D1400" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E1400" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1400" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1400" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1400" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1400" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1400" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1400" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>Failure To Reinstate License Ucm 1-2/3yrs</t>
+        </is>
+      </c>
+      <c r="D1401" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E1401" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1401" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1401" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1401" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1401" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1401" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1401" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>Failure To File Registration</t>
+        </is>
+      </c>
+      <c r="D1402" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E1402" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F1402" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G1402" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1402" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1402" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1402" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1402" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>DUS Ucm</t>
+        </is>
+      </c>
+      <c r="D1403" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E1403" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1403" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1403" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1403" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1403" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>Operating W/o A Valid Ol - Ucm</t>
+        </is>
+      </c>
+      <c r="D1404" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E1404" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1404" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1404" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1404" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1404" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>Failure To Reinstate License Ucm 1-2/3yrs</t>
+        </is>
+      </c>
+      <c r="D1405" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E1405" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1405" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1405" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1405" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1405" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>Failure To File Registration</t>
+        </is>
+      </c>
+      <c r="D1406" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E1406" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F1406" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1406" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1406" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1406" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>DUS Ucm</t>
+        </is>
+      </c>
+      <c r="D1407" t="inlineStr">
+        <is>
+          <t>4510.111</t>
+        </is>
+      </c>
+      <c r="E1407" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1407" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1407" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1407" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1407" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1407" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1407" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>Operating W/o A Valid Ol - Ucm</t>
+        </is>
+      </c>
+      <c r="D1408" t="inlineStr">
+        <is>
+          <t>4510.12</t>
+        </is>
+      </c>
+      <c r="E1408" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1408" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1408" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1408" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1408" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1408" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1408" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>Failure To Reinstate License Ucm 1-2/3yrs</t>
+        </is>
+      </c>
+      <c r="D1409" t="inlineStr">
+        <is>
+          <t>4510.21A*</t>
+        </is>
+      </c>
+      <c r="E1409" t="inlineStr">
+        <is>
+          <t>UCM</t>
+        </is>
+      </c>
+      <c r="F1409" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1409" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1409" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1409" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1409" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1409" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>21TRD09200</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Bunner</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>Failure To File Registration</t>
+        </is>
+      </c>
+      <c r="D1410" t="inlineStr">
+        <is>
+          <t>4503.11</t>
+        </is>
+      </c>
+      <c r="E1410" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F1410" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G1410" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="H1410" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="I1410" t="inlineStr">
+        <is>
+          <t>$ 0</t>
+        </is>
+      </c>
+      <c r="J1410" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="K1410" t="inlineStr">
         <is>
           <t>None</t>
         </is>

</xml_diff>